<commit_message>
update catalog builder tutorial
</commit_message>
<xml_diff>
--- a/tests/sample_tests_data/data/station/station.xlsx
+++ b/tests/sample_tests_data/data/station/station.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\station\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lqt-moment-magnitude\tests\sample_tests_data\data\station\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1F9925-982B-4791-8BAE-5F542FA4AFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A67CEED-B16A-485B-94B9-BE483D92E32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>KJ01</t>
   </si>
@@ -415,7 +426,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -424,7 +435,7 @@
     <col min="7" max="7" width="12.59765625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -438,7 +449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -451,11 +462,8 @@
       <c r="D2">
         <v>1120</v>
       </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -468,11 +476,8 @@
       <c r="D3">
         <v>1496</v>
       </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -485,11 +490,8 @@
       <c r="D4">
         <v>1335</v>
       </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -502,11 +504,8 @@
       <c r="D5">
         <v>1571</v>
       </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -519,11 +518,8 @@
       <c r="D6">
         <v>1150</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -536,11 +532,8 @@
       <c r="D7">
         <v>1396</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -553,11 +546,8 @@
       <c r="D8">
         <v>1112</v>
       </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -570,11 +560,8 @@
       <c r="D9">
         <v>1151</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -587,11 +574,8 @@
       <c r="D10">
         <v>1270</v>
       </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -604,11 +588,8 @@
       <c r="D11">
         <v>1220</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -621,11 +602,8 @@
       <c r="D12">
         <v>1312</v>
       </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -638,11 +616,8 @@
       <c r="D13">
         <v>989</v>
       </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -655,11 +630,8 @@
       <c r="D14">
         <v>1222</v>
       </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -672,11 +644,8 @@
       <c r="D15">
         <v>1398</v>
       </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -688,9 +657,6 @@
       </c>
       <c r="D16">
         <v>953</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>